<commit_message>
Final state Status Bericht 1
</commit_message>
<xml_diff>
--- a/20-11-23_Statusbericht/20-11-20_Barometer.xlsx
+++ b/20-11-23_Statusbericht/20-11-20_Barometer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\AAA_Studium_HAW_Mechatronik\WiSe20\Bachelorprojekt\bachelorprojekt2020\20-11-23_Statusbericht\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F183FAA-96B1-49E1-BE47-4A3BE9527B7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EE8830-36E3-44F3-A6F6-C9426824FFEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BDADFF32-FBD9-4DE5-B950-468D92E439C4}"/>
   </bookViews>
@@ -1968,98 +1968,103 @@
       <xdr:row>49</xdr:row>
       <xdr:rowOff>100853</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagramm 2">
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="4" name="Gruppieren 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2218D692-9CA0-4687-84DA-C8B4C4BD72B4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEBF1EAF-B4FE-458E-9087-590E9E24D537}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>331237</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>19915</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>219177</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>42327</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Sprechblase: rechteckig 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D34716B-09CC-44F8-A7DD-0512E7924E6C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4107619" y="5959033"/>
-          <a:ext cx="2173940" cy="784412"/>
+          <a:off x="1490382" y="5805767"/>
+          <a:ext cx="11261912" cy="3853704"/>
+          <a:chOff x="1490382" y="5805767"/>
+          <a:chExt cx="11261912" cy="3853704"/>
         </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -154116"/>
-            <a:gd name="adj2" fmla="val -2284"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1100"/>
-            <a:t>Beim ersten Meeting herrschte eine hohe</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
-            <a:t> Motivation, gleichzeitig aber auch die geringste Strukturiertheit        </a:t>
-          </a:r>
-          <a:endParaRPr lang="de-DE" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+      </xdr:grpSpPr>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="3" name="Diagramm 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2218D692-9CA0-4687-84DA-C8B4C4BD72B4}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGraphicFramePr/>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="1490382" y="5805767"/>
+          <a:ext cx="11261912" cy="3853704"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="2" name="Sprechblase: rechteckig 1">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D34716B-09CC-44F8-A7DD-0512E7924E6C}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4107619" y="5959033"/>
+            <a:ext cx="2173940" cy="784412"/>
+          </a:xfrm>
+          <a:prstGeom prst="wedgeRectCallout">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val -154116"/>
+              <a:gd name="adj2" fmla="val -2284"/>
+            </a:avLst>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1100"/>
+              <a:t>Beim ersten Meeting herrschte eine hohe</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+              <a:t> Motivation, gleichzeitig aber auch die geringste Strukturiertheit        </a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2365,7 +2370,7 @@
   <dimension ref="A1:Z36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V34" sqref="V34"/>
+      <selection activeCell="W41" sqref="W41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>